<commit_message>
Added an example printing Hello world, to measure the speed of printing Hello world.
</commit_message>
<xml_diff>
--- a/data/Analysis results.xlsx
+++ b/data/Analysis results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jperrin/Workspaces/Book/net.jgp.books.sparkWithJava.ch04/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{69C7F0A9-4ADB-5B40-8995-5FE1CF5D7335}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{48A6459F-37BE-DC45-A600-90A20B736E2C}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="24000" activeTab="1" xr2:uid="{F3FD4CC9-8027-2249-A179-E8E1DC3BF11D}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="24000" xr2:uid="{F3FD4CC9-8027-2249-A179-E8E1DC3BF11D}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="3" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="132">
   <si>
     <t>Creating a session ................. 1742</t>
   </si>
@@ -359,68 +359,77 @@
     <t>No transformation</t>
   </si>
   <si>
-    <t>5. Transformations  ................... 0</t>
-  </si>
-  <si>
     <t>Only column creation</t>
   </si>
   <si>
-    <t>1. Creating a session ................. 1918</t>
-  </si>
-  <si>
-    <t>2. Loading initial dataset ............ 3778</t>
-  </si>
-  <si>
-    <t>3. Building full dataset .............. 173</t>
-  </si>
-  <si>
-    <t>4. Clean-up ........................... 21</t>
-  </si>
-  <si>
-    <t>5. Transformations  ................... 275</t>
-  </si>
-  <si>
-    <t>6. Final action ....................... 52084</t>
-  </si>
-  <si>
-    <t>1. Creating a session ................. 1729</t>
-  </si>
-  <si>
-    <t>2. Loading initial dataset ............ 3359</t>
-  </si>
-  <si>
-    <t>3. Building full dataset .............. 63</t>
-  </si>
-  <si>
-    <t>4. Clean-up ........................... 13</t>
-  </si>
-  <si>
-    <t>5. Transformations  ................... 196</t>
-  </si>
-  <si>
-    <t>6. Final action ....................... 72220</t>
-  </si>
-  <si>
-    <t>1. Creating a session ................. 1596</t>
-  </si>
-  <si>
-    <t>2. Loading initial dataset ............ 3352</t>
-  </si>
-  <si>
-    <t>3. Building full dataset .............. 56</t>
-  </si>
-  <si>
-    <t>4. Clean-up ........................... 11</t>
-  </si>
-  <si>
-    <t>6. Final action ....................... 51149</t>
+    <t>5. Transformations  ................ 0</t>
+  </si>
+  <si>
+    <t>mvn exec:exec</t>
+  </si>
+  <si>
+    <t>mvn exec:exec -DexecMode=COL</t>
+  </si>
+  <si>
+    <t>5. Transformations  ................ 182</t>
+  </si>
+  <si>
+    <t>mvn exec:exec -DexecMode=FULL</t>
+  </si>
+  <si>
+    <t>1. Creating a session .............. 1791</t>
+  </si>
+  <si>
+    <t>2. Loading initial dataset ......... 3287</t>
+  </si>
+  <si>
+    <t>3. Building full dataset ........... 242</t>
+  </si>
+  <si>
+    <t>4. Clean-up ........................ 8</t>
+  </si>
+  <si>
+    <t>6. Final action .................... 20770</t>
+  </si>
+  <si>
+    <t># of records ....................... 2487641</t>
+  </si>
+  <si>
+    <t>1. Creating a session .............. 1553</t>
+  </si>
+  <si>
+    <t>2. Loading initial dataset ......... 3197</t>
+  </si>
+  <si>
+    <t>3. Building full dataset ........... 208</t>
+  </si>
+  <si>
+    <t>6. Final action .................... 34061</t>
+  </si>
+  <si>
+    <t>1. Creating a session .............. 1903</t>
+  </si>
+  <si>
+    <t>2. Loading initial dataset ......... 3184</t>
+  </si>
+  <si>
+    <t>3. Building full dataset ........... 213</t>
+  </si>
+  <si>
+    <t>5. Transformations  ................ 205</t>
+  </si>
+  <si>
+    <t>6. Final action .................... 24909</t>
+  </si>
+  <si>
+    <t>Total processing time (excluding loading)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -457,6 +466,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Monaco"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -490,7 +505,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -517,6 +532,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Heading 1" xfId="1" builtinId="16" customBuiltin="1"/>
@@ -832,10 +849,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CADA2CDE-3D0A-F94A-9A37-5A88A2E00234}">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -843,207 +860,247 @@
     <col min="1" max="1" width="57.83203125" customWidth="1"/>
     <col min="3" max="3" width="57.83203125" customWidth="1"/>
     <col min="5" max="5" width="57.83203125" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="8" customFormat="1" ht="22" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="8" customFormat="1" ht="22" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>109</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E1" s="8" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+    <row r="2" spans="1:8" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="B4">
+        <f>INT(RIGHT(A4,LEN(A4)-FIND("@",SUBSTITUTE(A4,".","@",LEN(A4)-LEN(SUBSTITUTE(A4,".",""))),1)-1))</f>
+        <v>1791</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="D4">
+        <f>INT(RIGHT(C4,LEN(C4)-FIND("@",SUBSTITUTE(C4,".","@",LEN(C4)-LEN(SUBSTITUTE(C4,".",""))),1)-1))</f>
+        <v>1553</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="F4">
+        <f>INT(RIGHT(E4,LEN(E4)-FIND("@",SUBSTITUTE(E4,".","@",LEN(E4)-LEN(SUBSTITUTE(E4,".",""))),1)-1))</f>
+        <v>1903</v>
+      </c>
+      <c r="H4">
+        <f>AVERAGE(F4,D4,B4)</f>
+        <v>1749</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="B5">
+        <f t="shared" ref="B5:B10" si="0">INT(RIGHT(A5,LEN(A5)-FIND("@",SUBSTITUTE(A5,".","@",LEN(A5)-LEN(SUBSTITUTE(A5,".",""))),1)-1))</f>
+        <v>3287</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="D5">
+        <f t="shared" ref="D5:D10" si="1">INT(RIGHT(C5,LEN(C5)-FIND("@",SUBSTITUTE(C5,".","@",LEN(C5)-LEN(SUBSTITUTE(C5,".",""))),1)-1))</f>
+        <v>3197</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="F5">
+        <f t="shared" ref="F5:F10" si="2">INT(RIGHT(E5,LEN(E5)-FIND("@",SUBSTITUTE(E5,".","@",LEN(E5)-LEN(SUBSTITUTE(E5,".",""))),1)-1))</f>
+        <v>3184</v>
+      </c>
+      <c r="H5" s="13">
+        <f>AVERAGE(F5,D5,B5)</f>
+        <v>3222.6666666666665</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="B6">
+        <f t="shared" si="0"/>
+        <v>242</v>
+      </c>
+      <c r="C6" s="12" t="s">
         <v>124</v>
       </c>
-      <c r="B3">
-        <f>INT(RIGHT(A3,LEN(A3)-FIND("@",SUBSTITUTE(A3,".","@",LEN(A3)-LEN(SUBSTITUTE(A3,".",""))),1)-1))</f>
-        <v>1596</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="D3">
-        <f>INT(RIGHT(C3,LEN(C3)-FIND("@",SUBSTITUTE(C3,".","@",LEN(C3)-LEN(SUBSTITUTE(C3,".",""))),1)-1))</f>
-        <v>1729</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="F3">
-        <f>INT(RIGHT(E3,LEN(E3)-FIND("@",SUBSTITUTE(E3,".","@",LEN(E3)-LEN(SUBSTITUTE(E3,".",""))),1)-1))</f>
-        <v>1918</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="B4">
-        <f t="shared" ref="B4" si="0">INT(RIGHT(A4,LEN(A4)-FIND("@",SUBSTITUTE(A4,".","@",LEN(A4)-LEN(SUBSTITUTE(A4,".",""))),1)-1))</f>
-        <v>3352</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="D4">
-        <f t="shared" ref="D4" si="1">INT(RIGHT(C4,LEN(C4)-FIND("@",SUBSTITUTE(C4,".","@",LEN(C4)-LEN(SUBSTITUTE(C4,".",""))),1)-1))</f>
-        <v>3359</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="F4">
-        <f t="shared" ref="F4:F8" si="2">INT(RIGHT(E4,LEN(E4)-FIND("@",SUBSTITUTE(E4,".","@",LEN(E4)-LEN(SUBSTITUTE(E4,".",""))),1)-1))</f>
-        <v>3778</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="B5">
-        <f t="shared" ref="B5" si="3">INT(RIGHT(A5,LEN(A5)-FIND("@",SUBSTITUTE(A5,".","@",LEN(A5)-LEN(SUBSTITUTE(A5,".",""))),1)-1))</f>
-        <v>56</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="D5">
-        <f t="shared" ref="D5" si="4">INT(RIGHT(C5,LEN(C5)-FIND("@",SUBSTITUTE(C5,".","@",LEN(C5)-LEN(SUBSTITUTE(C5,".",""))),1)-1))</f>
-        <v>63</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="F5">
-        <f t="shared" si="2"/>
-        <v>173</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="B6">
-        <f t="shared" ref="B6" si="5">INT(RIGHT(A6,LEN(A6)-FIND("@",SUBSTITUTE(A6,".","@",LEN(A6)-LEN(SUBSTITUTE(A6,".",""))),1)-1))</f>
-        <v>11</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>121</v>
-      </c>
       <c r="D6">
-        <f t="shared" ref="D6" si="6">INT(RIGHT(C6,LEN(C6)-FIND("@",SUBSTITUTE(C6,".","@",LEN(C6)-LEN(SUBSTITUTE(C6,".",""))),1)-1))</f>
-        <v>13</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>115</v>
+        <f t="shared" si="1"/>
+        <v>208</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>128</v>
       </c>
       <c r="F6">
         <f t="shared" si="2"/>
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>110</v>
+        <v>213</v>
+      </c>
+      <c r="H6" s="13">
+        <f>AVERAGE(F6,D6,B6)</f>
+        <v>221</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="12" t="s">
+        <v>119</v>
       </c>
       <c r="B7">
-        <f t="shared" ref="B7" si="7">INT(RIGHT(A7,LEN(A7)-FIND("@",SUBSTITUTE(A7,".","@",LEN(A7)-LEN(SUBSTITUTE(A7,".",""))),1)-1))</f>
-        <v>0</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>122</v>
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>119</v>
       </c>
       <c r="D7">
-        <f t="shared" ref="D7" si="8">INT(RIGHT(C7,LEN(C7)-FIND("@",SUBSTITUTE(C7,".","@",LEN(C7)-LEN(SUBSTITUTE(C7,".",""))),1)-1))</f>
-        <v>196</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>116</v>
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>119</v>
       </c>
       <c r="F7">
         <f t="shared" si="2"/>
-        <v>275</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="B8">
-        <f t="shared" ref="B8" si="9">INT(RIGHT(A8,LEN(A8)-FIND("@",SUBSTITUTE(A8,".","@",LEN(A8)-LEN(SUBSTITUTE(A8,".",""))),1)-1))</f>
-        <v>51149</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="D8">
-        <f t="shared" ref="D8" si="10">INT(RIGHT(C8,LEN(C8)-FIND("@",SUBSTITUTE(C8,".","@",LEN(C8)-LEN(SUBSTITUTE(C8,".",""))),1)-1))</f>
-        <v>72220</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="F8">
+        <v>8</v>
+      </c>
+      <c r="H7" s="13">
+        <f>AVERAGE(F7,D7,B7)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="12"/>
+      <c r="C8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="H8" s="13">
+        <f>SUM(H4:H7)</f>
+        <v>5200.6666666666661</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="B9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="1"/>
+        <v>182</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>129</v>
+      </c>
+      <c r="F9">
         <f t="shared" si="2"/>
-        <v>52084</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B9" s="3">
-        <f>SUM(B3:B8)</f>
-        <v>56164</v>
-      </c>
-      <c r="D9" s="3">
-        <f>SUM(D3:D8)</f>
-        <v>77580</v>
-      </c>
-      <c r="F9" s="3">
-        <f>SUM(F3:F8)</f>
-        <v>58249</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>25</v>
+        <v>205</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="12" t="s">
+        <v>120</v>
       </c>
       <c r="B10">
-        <f t="shared" ref="B10" si="11">INT(RIGHT(A10,LEN(A10)-FIND("@",SUBSTITUTE(A10,".","@",LEN(A10)-LEN(SUBSTITUTE(A10,".",""))),1)-1))</f>
-        <v>5219968</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>25</v>
+        <f t="shared" si="0"/>
+        <v>20770</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>125</v>
       </c>
       <c r="D10">
-        <f t="shared" ref="D10" si="12">INT(RIGHT(C10,LEN(C10)-FIND("@",SUBSTITUTE(C10,".","@",LEN(C10)-LEN(SUBSTITUTE(C10,".",""))),1)-1))</f>
-        <v>5219968</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>25</v>
+        <f t="shared" si="1"/>
+        <v>34061</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>130</v>
       </c>
       <c r="F10">
-        <f t="shared" ref="F10" si="13">INT(RIGHT(E10,LEN(E10)-FIND("@",SUBSTITUTE(E10,".","@",LEN(E10)-LEN(SUBSTITUTE(E10,".",""))),1)-1))</f>
-        <v>5219968</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B11">
-        <f>B10/B9</f>
-        <v>92.941528381169434</v>
-      </c>
-      <c r="D11">
-        <f>D10/D9</f>
-        <v>67.284970353183809</v>
-      </c>
-      <c r="F11">
-        <f>F10/F9</f>
-        <v>89.614722999536468</v>
+        <f t="shared" si="2"/>
+        <v>24909</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>131</v>
+      </c>
+      <c r="B11" s="3">
+        <f>SUM(B6:B10)</f>
+        <v>21020</v>
+      </c>
+      <c r="D11" s="3">
+        <f>SUM(D6:D10)</f>
+        <v>34459</v>
+      </c>
+      <c r="F11" s="3">
+        <f>SUM(F6:F10)</f>
+        <v>25335</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="B12">
+        <f t="shared" ref="B12" si="3">INT(RIGHT(A12,LEN(A12)-FIND("@",SUBSTITUTE(A12,".","@",LEN(A12)-LEN(SUBSTITUTE(A12,".",""))),1)-1))</f>
+        <v>2487641</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="D12">
+        <f t="shared" ref="D12" si="4">INT(RIGHT(C12,LEN(C12)-FIND("@",SUBSTITUTE(C12,".","@",LEN(C12)-LEN(SUBSTITUTE(C12,".",""))),1)-1))</f>
+        <v>2487641</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="F12">
+        <f t="shared" ref="F12" si="5">INT(RIGHT(E12,LEN(E12)-FIND("@",SUBSTITUTE(E12,".","@",LEN(E12)-LEN(SUBSTITUTE(E12,".",""))),1)-1))</f>
+        <v>2487641</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B13">
+        <f>B12/B11</f>
+        <v>118.34638439581352</v>
+      </c>
+      <c r="D13">
+        <f>D12/D11</f>
+        <v>72.191328825560817</v>
+      </c>
+      <c r="F13">
+        <f>F12/F11</f>
+        <v>98.189895401618315</v>
       </c>
     </row>
   </sheetData>
@@ -1055,7 +1112,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F66573CD-5081-0847-88CD-3D545484E608}">
   <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>

</xml_diff>